<commit_message>
udpate of code b/4 approvals
</commit_message>
<xml_diff>
--- a/shared/Stream-Site-Management.xlsx
+++ b/shared/Stream-Site-Management.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="70">
   <si>
     <t>Whirlpool Wireframe</t>
   </si>
@@ -201,20 +201,38 @@
     <t>Sophie Web Property</t>
   </si>
   <si>
-    <t>Sophie Portal</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>shutdown</t>
+  </si>
+  <si>
+    <t>insurance.morerewards.ca</t>
+  </si>
+  <si>
+    <t>property.insurance.morerewards.ca</t>
+  </si>
+  <si>
+    <t>Sophie Portal/Main site</t>
+  </si>
+  <si>
+    <t>css upgradeable?</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>*Y-tweaks needed</t>
+  </si>
+  <si>
+    <t>*Y - CSS order is fixed in live</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +316,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -340,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -387,6 +416,28 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -690,29 +741,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="45.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="36.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="62.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="15.5703125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="62.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="34.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -735,19 +787,22 @@
         <v>20</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
@@ -766,14 +821,15 @@
       <c r="G2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="H2" s="20"/>
+      <c r="K2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>56</v>
       </c>
@@ -792,14 +848,17 @@
       <c r="G3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="H3" s="26" t="s">
+        <v>69</v>
+      </c>
       <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="14">
         <v>1972</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -814,18 +873,19 @@
       <c r="G4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="H4" s="23"/>
+      <c r="K4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="25">
         <v>1975</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -840,18 +900,21 @@
       <c r="G5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="H5" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="25">
         <v>1978</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -869,14 +932,17 @@
       <c r="G6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="H6" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>15</v>
       </c>
@@ -895,14 +961,17 @@
       <c r="G7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="H7" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -910,7 +979,7 @@
         <v>1995</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>55</v>
@@ -921,14 +990,17 @@
       <c r="G8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="H8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
@@ -936,7 +1008,7 @@
         <v>2062</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>40</v>
@@ -947,14 +1019,17 @@
       <c r="G9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="H9" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
@@ -962,7 +1037,7 @@
         <v>2064</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>40</v>
@@ -973,14 +1048,17 @@
       <c r="G10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="H10" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
@@ -991,7 +1069,7 @@
         <v>40</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>39</v>
@@ -999,14 +1077,17 @@
       <c r="G11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="H11" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
@@ -1025,14 +1106,17 @@
       <c r="G12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="H12" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>4</v>
       </c>
@@ -1051,21 +1135,24 @@
       <c r="G13" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="H13" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="K13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="14">
         <v>2080</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1083,21 +1170,22 @@
       <c r="G14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="23"/>
+      <c r="I14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="14">
         <v>2081</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1112,21 +1200,24 @@
       <c r="G15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="14">
         <v>2083</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1141,28 +1232,31 @@
       <c r="G16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2">
         <v>2084</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>40</v>
+      <c r="C17" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>57</v>
@@ -1170,17 +1264,20 @@
       <c r="G17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="K17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="L17" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1288,7 @@
         <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>50</v>
@@ -1199,28 +1296,31 @@
       <c r="G18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="H18" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="K18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="L18" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="2">
         <v>2087</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>40</v>
+      <c r="C19" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>57</v>
@@ -1228,10 +1328,13 @@
       <c r="G19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="H19" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="L19" s="6" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finalize mac-safari accordion highlight
</commit_message>
<xml_diff>
--- a/shared/Stream-Site-Management.xlsx
+++ b/shared/Stream-Site-Management.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="75">
   <si>
     <t>Whirlpool Wireframe</t>
   </si>
@@ -225,17 +225,29 @@
     <t>*Y-tweaks needed</t>
   </si>
   <si>
-    <t>*Y - CSS order is fixed in live</t>
-  </si>
-  <si>
-    <t>Shared CSS Nav?</t>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>More Rewads Site</t>
+  </si>
+  <si>
+    <t>http://www.digitalmarketingtest.com/index.php?ProductID=1970</t>
+  </si>
+  <si>
+    <t>Poweb Unique visitor ID</t>
+  </si>
+  <si>
+    <t>portal.insurance.morerewards.ca</t>
+  </si>
+  <si>
+    <t>/uploads/00001941/pcg-redesign-landing.css</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +292,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12.1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -287,58 +376,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <strike/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="9" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,8 +411,14 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -374,12 +441,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -390,9 +543,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -401,59 +551,174 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -757,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,645 +1033,711 @@
     <col min="1" max="1" width="32.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="21" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="40" style="3" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="62.7109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="34.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.42578125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" s="47" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="47" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="41">
         <v>1888</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="L2" s="5" t="s">
+      <c r="H2" s="51"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="52" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="17">
         <v>1970</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="17">
         <v>1972</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="L4" s="6" t="s">
+      <c r="H4" s="16"/>
+      <c r="L4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="17">
         <v>1975</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="L5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="17">
         <v>1978</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" s="5" t="s">
+      <c r="E6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="L6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="17">
         <v>1980</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="23" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="L7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="54">
+        <v>1995</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="60"/>
+      <c r="E8" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="54">
+        <v>2062</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="54">
+        <v>2064</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="60"/>
+      <c r="E10" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="20">
+        <v>2068</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L7" s="5" t="s">
+      <c r="F11" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M11" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1995</v>
-      </c>
-      <c r="C8" s="18" t="s">
+    <row r="12" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="63">
+        <v>2076</v>
+      </c>
+      <c r="C12" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="23" t="s">
+      <c r="D12" s="28"/>
+      <c r="E12" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="5" t="s">
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M12" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2062</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="23" t="s">
+    <row r="13" spans="1:13" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="32">
+        <v>2079</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="38"/>
+      <c r="E13" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="5" t="s">
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2064</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2068</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2076</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2079</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="25">
-        <v>2080</v>
+      <c r="B14" s="17">
+        <v>2091</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="E14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="L14" s="5" t="s">
+      <c r="H14" s="16"/>
+      <c r="J14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="28">
-        <v>2081</v>
+      <c r="B15" s="17">
+        <v>2093</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="5" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="J15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="28">
-        <v>2083</v>
+      <c r="B16" s="17">
+        <v>2094</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="5" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="J16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="2">
         <v>2084</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="41">
+        <v>2085</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="23" t="s">
+      <c r="F18" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L17" s="6" t="s">
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M18" s="46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2085</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="9" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="2">
         <v>2087</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="5" t="s">
+      <c r="D19" s="3"/>
+      <c r="E19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="H19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="M19" s="5" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2095</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2092</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2096</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D23" s="65"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D24" s="65"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D25" s="65"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>